<commit_message>
language stats final version
</commit_message>
<xml_diff>
--- a/language_stats.xlsx
+++ b/language_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,63 +453,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>delta</t>
+          <t>schaumburgernachrichten</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ja</t>
+          <t>en</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ponpon_</t>
+          <t>rff</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>fi</t>
+        </is>
+      </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>lain</t>
+          <t>MinnaRuokonen</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>de</t>
+          <t>pt</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>diaeter</t>
+          <t>g1_globo</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>da</t>
+          <t>th</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -517,29 +521,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MachoManPierreCardin</t>
+          <t>ogataquotes_th</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>ja</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Blaveur</t>
+          <t>osame120</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ru</t>
+          <t>es</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -547,7 +551,48 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Razunter</t>
+          <t>MelchorRuizCope</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>elysion</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>tr</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>tramboline</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>zh</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>tiefraum</t>
         </is>
       </c>
     </row>

</xml_diff>